<commit_message>
Timed and Untimed Practice Trials
Complete working example of timed and untimed practice
trials.  No counterbalancing yet, fixed expected response.
</commit_message>
<xml_diff>
--- a/exp/task-switching-replication-trialtypes.xlsx
+++ b/exp/task-switching-replication-trialtypes.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="18">
   <si>
     <t xml:space="preserve">cueType</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t xml:space="preserve">targetFileName</t>
+  </si>
+  <si>
+    <t xml:space="preserve">correctAnswer</t>
   </si>
   <si>
     <t xml:space="preserve">dashed</t>
@@ -167,13 +170,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="F11" activeCellId="0" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24.73"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="34.18"/>
@@ -195,141 +198,168 @@
       <c r="E1" s="0" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F3" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F4" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
+      </c>
+      <c r="F6" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="0" t="s">
         <v>15</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>14</v>
+      <c r="F9" s="0" t="n">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>